<commit_message>
refactor: auth badge button collapse dialog divider style: layout
</commit_message>
<xml_diff>
--- a/src/i18n/i18n.xlsx
+++ b/src/i18n/i18n.xlsx
@@ -24,11 +24,11 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="AJ篩選 非本人勿用" guid="{26C905C7-2C39-4702-9479-6A8F4386ED3B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="篩選器 2" guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="AJ篩選 非本人勿用" guid="{26C905C7-2C39-4702-9479-6A8F4386ED3B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -174,10 +174,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Excel系統</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Excel測試</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -207,6 +203,10 @@
   </si>
   <si>
     <t>ExcelPage</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel系統123</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -649,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -887,13 +887,13 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -920,13 +920,13 @@
         <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -953,13 +953,13 @@
         <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1235,30 +1235,18 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="E1:E907"/>
+      <autoFilter ref="A2:AA913">
+        <filterColumn colId="3">
+          <filters>
+            <filter val="V"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:I613"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:N612"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -1279,18 +1267,30 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:AA913">
-        <filterColumn colId="3">
-          <filters>
-            <filter val="V"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="A1:N612"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="A2:I613"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="E1:E907"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -1332,6 +1332,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097749175EA382F46998456ACE2E5E022" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f9564bd998978afe117d271aa86623d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="656db63e-0aa2-4982-a6ef-7cfc894502dc" xmlns:ns3="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c8d268a87e81341ebbd7ca6aba28788" ns2:_="" ns3:_="">
     <xsd:import namespace="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
@@ -1542,17 +1553,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1563,6 +1563,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
+    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B5B63AB-5528-472F-BE4A-13B18B02B409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1581,17 +1592,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
-    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{043FBB36-7F63-4B63-8343-64EBAA2E147B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
refactor: i18n + globalView fix: input oprator
</commit_message>
<xml_diff>
--- a/src/i18n/i18n.xlsx
+++ b/src/i18n/i18n.xlsx
@@ -24,11 +24,11 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="篩選器 2" guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="AJ篩選 非本人勿用" guid="{26C905C7-2C39-4702-9479-6A8F4386ED3B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 2" guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -115,14 +115,6 @@
   </si>
   <si>
     <t>系统</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -649,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -708,12 +700,8 @@
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
@@ -743,14 +731,10 @@
     <row r="3" spans="1:21" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,7 +764,7 @@
     <row r="4" spans="1:21" ht="15.75" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -814,20 +798,20 @@
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -848,19 +832,19 @@
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -884,16 +868,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -917,16 +901,16 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -950,16 +934,16 @@
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1235,18 +1219,30 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:AA913">
-        <filterColumn colId="3">
-          <filters>
-            <filter val="V"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="E1:E907"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="A2:I613"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="A1:N612"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -1267,30 +1263,18 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:N612"/>
+      <autoFilter ref="A2:AA913">
+        <filterColumn colId="3">
+          <filters>
+            <filter val="V"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:I613"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="E1:E907"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -1332,17 +1316,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097749175EA382F46998456ACE2E5E022" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f9564bd998978afe117d271aa86623d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="656db63e-0aa2-4982-a6ef-7cfc894502dc" xmlns:ns3="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c8d268a87e81341ebbd7ca6aba28788" ns2:_="" ns3:_="">
     <xsd:import namespace="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
@@ -1553,6 +1526,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1563,17 +1547,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
-    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B5B63AB-5528-472F-BE4A-13B18B02B409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1592,6 +1565,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
+    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{043FBB36-7F63-4B63-8343-64EBAA2E147B}">
   <ds:schemaRefs>

</xml_diff>